<commit_message>
Add new U1 panelized production files
</commit_message>
<xml_diff>
--- a/without-power-switch/U1_SMD/U1_BOM.xlsx
+++ b/without-power-switch/U1_SMD/U1_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\unified-daughterboard-with-power-switch\without-power-switch\U1_SMD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\unified-daughterboard\without-power-switch\U1_SMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD1DC7A-8ED7-4D72-A4D9-571AC1062F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="7260" yWindow="1890" windowWidth="24420" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,31 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>值/型号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>封装</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1k</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>USBLC6-2P6</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,22 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.usb.org/sites/default/files/documents/usb_type-c.zip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.st.com/resource/en/datasheet/usblc6-2.pdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>R1, R2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,13 +67,69 @@
   </si>
   <si>
     <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位号/Designator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1kΩ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>封装/Footprint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量/Quantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注/Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>型号/Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16Pin Type-C母座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH 4Pin端子插座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5%贴片电阻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESD芯片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘉立创元件编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C709357</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2764183</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2827693</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,16 +287,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,22 +305,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -585,106 +602,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="39.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="57.25" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="35.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="48.6328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31.26953125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="39.81640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>11</v>
+      <c r="F5" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>